<commit_message>
import file and validate order's data from excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/ListOrder.xlsx
+++ b/src/main/resources/templates/ListOrder.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
   <si>
     <t>nameSender</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>djsjdjasjdj2@gmail.com</t>
+  </si>
+  <si>
+    <t>098274</t>
+  </si>
+  <si>
+    <t>sdsadsadasdsa.com</t>
+  </si>
+  <si>
+    <t>tttt</t>
   </si>
 </sst>
 </file>
@@ -200,117 +209,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -761,7 +660,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:J6"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,7 +714,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>11</v>
@@ -843,9 +742,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -885,7 +782,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>13</v>
@@ -923,7 +820,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>15</v>
@@ -967,7 +864,7 @@
         <v>34</v>
       </c>
       <c r="J6" s="7">
-        <v>55</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1056,43 +953,43 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8:C13">
-    <cfRule type="duplicateValues" dxfId="25" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="24" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="duplicateValues" dxfId="20" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B13">
-    <cfRule type="duplicateValues" dxfId="19" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="18" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="14" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="13" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="12" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
@@ -1114,13 +1011,13 @@
     <hyperlink ref="D3" r:id="rId6"/>
     <hyperlink ref="E4" r:id="rId7" display="hahhdh@gmail.com"/>
     <hyperlink ref="H4" r:id="rId8"/>
-    <hyperlink ref="D4" r:id="rId9"/>
-    <hyperlink ref="E5" r:id="rId10" display="hahhdh@gmail.com"/>
-    <hyperlink ref="H5" r:id="rId11"/>
-    <hyperlink ref="D5" r:id="rId12"/>
-    <hyperlink ref="E6" r:id="rId13" display="hahhdh@gmail.com"/>
-    <hyperlink ref="H6" r:id="rId14"/>
-    <hyperlink ref="D6" r:id="rId15"/>
+    <hyperlink ref="E5" r:id="rId9" display="hahhdh@gmail.com"/>
+    <hyperlink ref="H5" r:id="rId10"/>
+    <hyperlink ref="D5" r:id="rId11"/>
+    <hyperlink ref="E6" r:id="rId12" display="hahhdh@gmail.com"/>
+    <hyperlink ref="H6" r:id="rId13"/>
+    <hyperlink ref="D6" r:id="rId14"/>
+    <hyperlink ref="D4" r:id="rId15" display="hahhdh@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>

</xml_diff>